<commit_message>
Análise de retenção de IR sendo feita e adicionada no arquivo xlsx (Excel). Provavelmente terá que ser refinada.
</commit_message>
<xml_diff>
--- a/output_data.xlsx
+++ b/output_data.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -425,6 +425,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="11" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -438,6 +439,11 @@
           <t>Renteção de ISS</t>
         </is>
       </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Retenção IR</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -448,6 +454,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -458,6 +469,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="C3" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -468,6 +484,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="C4" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -478,6 +499,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="C5" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -488,6 +514,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="C6" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -498,6 +529,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="C7" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -508,6 +544,11 @@
           <t>X</t>
         </is>
       </c>
+      <c r="C8" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -518,6 +559,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="C9" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -528,6 +574,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="C10" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -538,6 +589,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="C11" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -548,6 +604,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="C12" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -558,6 +619,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="C13" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -568,6 +634,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="C14" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -578,6 +649,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="C15" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -588,6 +664,11 @@
           <t>X</t>
         </is>
       </c>
+      <c r="C16" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -598,6 +679,15 @@
           <t>-</t>
         </is>
       </c>
+      <c r="C17" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" s="1" t="n"/>
+      <c r="C18" s="1" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Análise de retenção de CSRF sendo feita.
</commit_message>
<xml_diff>
--- a/output_data.xlsx
+++ b/output_data.xlsx
@@ -46,10 +46,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -416,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,270 +427,1400 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="15" customWidth="1" min="2" max="2"/>
-    <col width="11" customWidth="1" min="3" max="3"/>
+    <col width="10" customWidth="1" min="1" max="1"/>
+    <col width="22" customWidth="1" min="2" max="2"/>
+    <col width="24" customWidth="1" min="3" max="3"/>
+    <col width="17" customWidth="1" min="4" max="4"/>
+    <col width="13" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Notas</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
+          <t>Nota</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Razão Social Tomador</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Razão Social Prestador</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Renteção de ISS</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Retenção IR</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Retenção CSRF</t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="A2" s="2" t="n">
         <v>31</v>
       </c>
-      <c r="B2" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C2" s="1" t="inlineStr">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Macnica Dhw Ltda</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>FRANCIELE NORNBERG</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E2" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F2" s="1" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" s="2" t="n">
         <v>15</v>
       </c>
-      <c r="B3" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C3" s="1" t="inlineStr">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ESPACO PRIME COMERCIO DE BEBIDAS E DELICATESSEN LTDA</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>LNA PROMOCAO DE VENDAS LTDA</t>
+        </is>
+      </c>
+      <c r="D3" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E3" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F3" s="1" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
+      <c r="A4" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="B4" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C4" s="1" t="inlineStr">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>MACNICA DHW LTDA</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>MARINA SIQUEIRA PETRASSEM SOUSA 08896969930</t>
+        </is>
+      </c>
+      <c r="D4" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E4" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F4" s="1" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" s="2" t="n">
         <v>32</v>
       </c>
-      <c r="B5" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C5" s="1" t="inlineStr">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>MACNICA DHW LTDA.</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>HAZAEL DOS SANTOS BATISTA</t>
+        </is>
+      </c>
+      <c r="D5" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E5" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F5" s="1" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" s="2" t="n">
         <v>2950</v>
       </c>
-      <c r="B6" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C6" s="1" t="inlineStr">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>B&amp;C CONSULTORIA LTDA</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>MARIO DE ALMEIDA E ANTONINI PROP INTEL LTDA</t>
+        </is>
+      </c>
+      <c r="D6" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E6" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F6" s="1" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
+      <c r="A7" s="2" t="n">
         <v>227715</v>
       </c>
-      <c r="B7" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C7" s="1" t="inlineStr">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>CLINICA CARDIOSPORT DE PREV E REAB LTDA</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>AHGORA SISTEMAS S.A.</t>
+        </is>
+      </c>
+      <c r="D7" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E7" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F7" s="1" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
+      <c r="A8" s="2" t="n">
         <v>6436</v>
       </c>
-      <c r="B8" s="1" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C8" s="1" t="inlineStr">
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>ARTHUR SILVEIRA CONSTRUTORA E INCORPORADORA LTDA</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>CIA DE CIMENTO ITAMBE</t>
+        </is>
+      </c>
+      <c r="D8" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E8" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F8" s="1" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
+      <c r="A9" s="2" t="n">
         <v>55</v>
       </c>
-      <c r="B9" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C9" s="1" t="inlineStr">
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>MACNICA DHW LTDA</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>WILLIAM SIMON GUTSTEIN 04189596922</t>
+        </is>
+      </c>
+      <c r="D9" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E9" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F9" s="1" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
+      <c r="A10" s="2" t="n">
         <v>44319</v>
       </c>
-      <c r="B10" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C10" s="1" t="inlineStr">
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Clinica Cardiosport de Prevencao e Reabilitacao S/C Ltda.</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>MANAGER CONSULTORIA EM INFORMATICA - EIRELI</t>
+        </is>
+      </c>
+      <c r="D10" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E10" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="F10" s="1" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
+      <c r="A11" s="2" t="n">
         <v>196</v>
       </c>
-      <c r="B11" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C11" s="1" t="inlineStr">
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Macnica DHW Ltda.</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>RODRIGUES ADVOCACIA E CONSULTORIA JURIDICA.</t>
+        </is>
+      </c>
+      <c r="D11" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E11" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F11" s="1" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="n">
+      <c r="A12" s="2" t="n">
         <v>152</v>
       </c>
-      <c r="B12" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C12" s="1" t="inlineStr">
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>MACNICA DHW LTDA</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>ND2ETEC - SERV DA TEC N DA INFORMACAO LTDA ME</t>
+        </is>
+      </c>
+      <c r="D12" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E12" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F12" s="1" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="n">
+      <c r="A13" s="2" t="n">
         <v>47632</v>
       </c>
-      <c r="B13" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C13" s="1" t="inlineStr">
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>MACNICA DHW LTDA</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>AMPLA SERVICOS MEDICOS LTDA</t>
+        </is>
+      </c>
+      <c r="D13" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E13" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F13" s="1" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="n">
+      <c r="A14" s="2" t="n">
         <v>9014</v>
       </c>
-      <c r="B14" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C14" s="1" t="inlineStr">
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>POSTAL SAÚDE - CAIXA DE ASSISTÊNCIA E SAÚDE DOS EMPREGADOS DOS CORREIOS</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>POLICLINICA SANTA CATARINA LTDA</t>
+        </is>
+      </c>
+      <c r="D14" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E14" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="F14" s="1" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="n">
+      <c r="A15" s="2" t="n">
+        <v>862</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>FUNDO ESTADUAL DE SAUDE</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>CIENCIA LABORATORIO MEDICO LTDA</t>
+        </is>
+      </c>
+      <c r="D15" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E15" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="F15" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="n">
+        <v>863</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>FUNDO ESTADUAL DE SAUDE</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>CIENCIA LABORATORIO MEDICO LTDA</t>
+        </is>
+      </c>
+      <c r="D16" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E16" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="F16" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="n">
+        <v>864</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>FUNDO ESTADUAL DE SAUDE</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>CIENCIA LABORATORIO MEDICO LTDA</t>
+        </is>
+      </c>
+      <c r="D17" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E17" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="F17" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="n">
+        <v>865</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>SESI SERVICO SOCIAL DA INDUSTRIA</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>CIENCIA LABORATORIO MEDICO LTDA</t>
+        </is>
+      </c>
+      <c r="D18" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E18" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="F18" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="n">
+        <v>866</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>BRADESCO SAUDE</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>CIENCIA LABORATORIO MEDICO LTDA</t>
+        </is>
+      </c>
+      <c r="D19" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E19" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="F19" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="n">
+        <v>867</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>SISREG FUNDO MUNICIPAL DE SAUDE DE FLORIANOPOLIS</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>CIENCIA LABORATORIO MEDICO LTDA</t>
+        </is>
+      </c>
+      <c r="D20" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E20" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="F20" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="n">
+        <v>868</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>SISREG FUNDO MUNICIPAL DE SAUDE DE FLORIANOPOLIS</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>CIENCIA LABORATORIO MEDICO LTDA</t>
+        </is>
+      </c>
+      <c r="D21" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E21" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="F21" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="n">
+        <v>869</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>SISREG FUNDO MUNICIPAL DE SAUDE DE FLORIANOPOLIS</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>CIENCIA LABORATORIO MEDICO LTDA</t>
+        </is>
+      </c>
+      <c r="D22" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E22" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="F22" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="n">
+        <v>870</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>ASSOCIACAO DE VOLUNTARIOS DE APOIO E ASSISTENCIA A CRIANCA E AO ADOLESCENTE</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>CIENCIA LABORATORIO MEDICO LTDA</t>
+        </is>
+      </c>
+      <c r="D23" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E23" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F23" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="n">
+        <v>871</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>SISREG FUNDO MUNICIPAL DE SAUDE DE FLORIANOPOLIS</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>CIENCIA LABORATORIO MEDICO LTDA</t>
+        </is>
+      </c>
+      <c r="D24" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E24" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="F24" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="n">
+        <v>872</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>SISREG FUNDO MUNICIPAL DE SAUDE DE FLORIANOPOLIS</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>CIENCIA LABORATORIO MEDICO LTDA</t>
+        </is>
+      </c>
+      <c r="D25" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E25" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="F25" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="n">
+        <v>873</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>SOCIEDADE LITERARIA E CARITATIVA SANTO AGOSTINHO - HOSPITAL SAO JOSE</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>CIENCIA LABORATORIO MEDICO LTDA</t>
+        </is>
+      </c>
+      <c r="D26" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E26" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F26" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="n">
+        <v>874</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>ASSOCIACAO DE VOLUNTARIOS DE APOIO E ASSISTENCIA A CRIANCA E AO ADOLESCENTE</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>CIENCIA LABORATORIO MEDICO LTDA</t>
+        </is>
+      </c>
+      <c r="D27" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E27" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F27" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="n">
+        <v>875</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>ELOSAUDE ASSOCIACAO DE ASSISTENCIA A SAUDE</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>CIENCIA LABORATORIO MEDICO LTDA</t>
+        </is>
+      </c>
+      <c r="D28" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E28" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F28" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="n">
+        <v>876</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>ASSOCIACAO DE VOLUNTARIOS DE APOIO E ASSISTENCIA A CRIANCA E AO ADOLESCENTE</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>CIENCIA LABORATORIO MEDICO LTDA</t>
+        </is>
+      </c>
+      <c r="D29" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E29" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F29" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="n">
+        <v>877</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>UNIMED GRANDE FLORIANOPOLIS COOPERATIVA DE TRABALHO MEDICO</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>CIENCIA LABORATORIO MEDICO LTDA</t>
+        </is>
+      </c>
+      <c r="D30" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E30" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="F30" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="n">
+        <v>878</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>FUNDO ESTADUAL DE SAUDE</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>CIENCIA LABORATORIO MEDICO LTDA</t>
+        </is>
+      </c>
+      <c r="D31" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E31" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="F31" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="2" t="n">
+        <v>880</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>FUNDO ESTADUAL DE SAUDE</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>CIENCIA LABORATORIO MEDICO LTDA</t>
+        </is>
+      </c>
+      <c r="D32" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E32" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="F32" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="2" t="n">
+        <v>881</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>SESI SERVICO SOCIAL DA INDUSTRIA</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>CIENCIA LABORATORIO MEDICO LTDA</t>
+        </is>
+      </c>
+      <c r="D33" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E33" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="F33" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="n">
+        <v>882</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>BRADESCO SAUDE</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>CIENCIA LABORATORIO MEDICO LTDA</t>
+        </is>
+      </c>
+      <c r="D34" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E34" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="F34" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="2" t="n">
+        <v>883</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>SISREG FUNDO MUNICIPAL DE SAUDE DE FLORIANOPOLIS</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>CIENCIA LABORATORIO MEDICO LTDA</t>
+        </is>
+      </c>
+      <c r="D35" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E35" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="F35" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="n">
+        <v>884</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>SISREG FUNDO MUNICIPAL DE SAUDE DE FLORIANOPOLIS</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>CIENCIA LABORATORIO MEDICO LTDA</t>
+        </is>
+      </c>
+      <c r="D36" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E36" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="F36" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="2" t="n">
+        <v>885</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>SOCIEDADE LITERARIA E CARITATIVA SANTO AGOSTINHO - HOSPITAL SAO JOSE</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>CIENCIA LABORATORIO MEDICO LTDA</t>
+        </is>
+      </c>
+      <c r="D37" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E37" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F37" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="2" t="n">
+        <v>886</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>ASSOCIACAO DE VOLUNTARIOS DE APOIO E ASSISTENCIA A CRIANCA E AO ADOLESCENTE</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>CIENCIA LABORATORIO MEDICO LTDA</t>
+        </is>
+      </c>
+      <c r="D38" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E38" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F38" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="2" t="n">
+        <v>887</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Toxicologia Pardini Laboratorios S/A</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>CIENCIA LABORATORIO MEDICO LTDA</t>
+        </is>
+      </c>
+      <c r="D39" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E39" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="F39" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="2" t="n">
+        <v>888</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>ELOSAUDE ASSOCIACAO DE ASSISTENCIA A SAUDE</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>CIENCIA LABORATORIO MEDICO LTDA</t>
+        </is>
+      </c>
+      <c r="D40" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E40" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="F40" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="2" t="n">
+        <v>889</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>ELOSAUDE ASSOCIACAO DE ASSISTENCIA A SAUDE</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>CIENCIA LABORATORIO MEDICO LTDA</t>
+        </is>
+      </c>
+      <c r="D41" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E41" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F41" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="2" t="n">
+        <v>890</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>BRADESCO SAUDE</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>CIENCIA LABORATORIO MEDICO LTDA</t>
+        </is>
+      </c>
+      <c r="D42" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E42" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="F42" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="2" t="n">
+        <v>891</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>UNIMED GRANDE FLORIANOPOLIS COOPERATIVA DE TRABALHO MEDICO</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>CIENCIA LABORATORIO MEDICO LTDA</t>
+        </is>
+      </c>
+      <c r="D43" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E43" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="F43" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="2" t="n">
         <v>1877</v>
       </c>
-      <c r="B15" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C15" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>MACNICA DHW LTDA</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>LIVTI TECNOLOGIA LTDA</t>
+        </is>
+      </c>
+      <c r="D44" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E44" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F44" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="2" t="n">
         <v>597</v>
       </c>
-      <c r="B16" s="1" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C16" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Macnica DHW ltda</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>PARAISO - AGENCIA DE VIAGENS E TURISMO LTDA.</t>
+        </is>
+      </c>
+      <c r="D45" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E45" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F45" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="2" t="n">
         <v>419</v>
       </c>
-      <c r="B17" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C17" s="1" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="B18" s="1" t="n"/>
-      <c r="C18" s="1" t="n"/>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>B&amp;C Consultoria Ltda.</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>A VERO DOMINO CONSULTORIA E PESQUISA LTDA</t>
+        </is>
+      </c>
+      <c r="D46" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E46" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="F46" s="1" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="D47" s="1" t="n"/>
+      <c r="E47" s="1" t="n"/>
+      <c r="F47" s="1" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>